<commit_message>
updated: fixed some bugs
</commit_message>
<xml_diff>
--- a/backend/excel-file/asad.xlsx
+++ b/backend/excel-file/asad.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M79"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3641,9 +3641,296 @@
         <v>21:55:00</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80">
+        <v>1119373171</v>
+      </c>
+      <c r="B80" t="str">
+        <v>212417459</v>
+      </c>
+      <c r="C80" t="str">
+        <v>ABDUL SATTAR</v>
+      </c>
+      <c r="D80" t="str">
+        <v>GHULAM AKBAR</v>
+      </c>
+      <c r="E80" t="str">
+        <v>LASHARI</v>
+      </c>
+      <c r="F80" t="str">
+        <v>4120263884305</v>
+      </c>
+      <c r="G80" t="str">
+        <v>B.B.A (HONS)</v>
+      </c>
+      <c r="H80" t="str">
+        <v>ANNUAL FEE</v>
+      </c>
+      <c r="I80" t="str">
+        <v>University of Sindh</v>
+      </c>
+      <c r="J80">
+        <v>42000</v>
+      </c>
+      <c r="K80" t="str">
+        <v>1BILL_PAY</v>
+      </c>
+      <c r="L80" t="str">
+        <v>2024-01-15T19:00:00.000Z</v>
+      </c>
+      <c r="M80" t="str">
+        <v>12:56:00</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>1119342229</v>
+      </c>
+      <c r="B81" t="str">
+        <v>212417457</v>
+      </c>
+      <c r="C81" t="str">
+        <v>ABDUL HAFEEZ</v>
+      </c>
+      <c r="D81" t="str">
+        <v>ASHIQUE HUSSAIN</v>
+      </c>
+      <c r="E81" t="str">
+        <v>SOOMRO</v>
+      </c>
+      <c r="F81" t="str">
+        <v>4120124622975</v>
+      </c>
+      <c r="G81" t="str">
+        <v>B.B.A (HONS)</v>
+      </c>
+      <c r="H81" t="str">
+        <v>ANNUAL FEE</v>
+      </c>
+      <c r="I81" t="str">
+        <v>University of Sindh</v>
+      </c>
+      <c r="J81">
+        <v>42000</v>
+      </c>
+      <c r="K81" t="str">
+        <v>1BILL_PAY</v>
+      </c>
+      <c r="L81" t="str">
+        <v>2024-01-15T19:00:00.000Z</v>
+      </c>
+      <c r="M81" t="str">
+        <v>12:19:00</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>1119358164</v>
+      </c>
+      <c r="B82" t="str">
+        <v>212402523</v>
+      </c>
+      <c r="C82" t="str">
+        <v>DUA</v>
+      </c>
+      <c r="D82" t="str">
+        <v>ZULFIQAR ALI</v>
+      </c>
+      <c r="E82" t="str">
+        <v>MEMON</v>
+      </c>
+      <c r="F82" t="str">
+        <v>4160106507616</v>
+      </c>
+      <c r="G82" t="str">
+        <v>B.B.A (HONS)</v>
+      </c>
+      <c r="H82" t="str">
+        <v>ANNUAL FEE</v>
+      </c>
+      <c r="I82" t="str">
+        <v>University of Sindh</v>
+      </c>
+      <c r="J82">
+        <v>42000</v>
+      </c>
+      <c r="K82" t="str">
+        <v>1BILL_PAY</v>
+      </c>
+      <c r="L82" t="str">
+        <v>2024-01-15T19:00:00.000Z</v>
+      </c>
+      <c r="M82" t="str">
+        <v>12:36:00</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>1119452756</v>
+      </c>
+      <c r="B83" t="str">
+        <v>212414137</v>
+      </c>
+      <c r="C83" t="str">
+        <v>SURAJ KUMAR</v>
+      </c>
+      <c r="D83" t="str">
+        <v>RAJESH KUMAR</v>
+      </c>
+      <c r="E83" t="str">
+        <v>MAHESHWARI</v>
+      </c>
+      <c r="F83" t="str">
+        <v>4440390471307</v>
+      </c>
+      <c r="G83" t="str">
+        <v>BS (COMPUTER SCIENCE) PRE-ENGINEERING</v>
+      </c>
+      <c r="H83" t="str">
+        <v>ANNUAL FEE</v>
+      </c>
+      <c r="I83" t="str">
+        <v>University of Sindh</v>
+      </c>
+      <c r="J83">
+        <v>42000</v>
+      </c>
+      <c r="K83" t="str">
+        <v>1BILL_PAY</v>
+      </c>
+      <c r="L83" t="str">
+        <v>2024-01-15T19:00:00.000Z</v>
+      </c>
+      <c r="M83" t="str">
+        <v>14:30:00</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>1119483553</v>
+      </c>
+      <c r="B84" t="str">
+        <v>212417462</v>
+      </c>
+      <c r="C84" t="str">
+        <v>ALI RAZA</v>
+      </c>
+      <c r="D84" t="str">
+        <v>GHULAM SARWAR</v>
+      </c>
+      <c r="E84" t="str">
+        <v>PANHWAR</v>
+      </c>
+      <c r="F84" t="str">
+        <v>4120189418207</v>
+      </c>
+      <c r="G84" t="str">
+        <v>B.B.A (HONS)</v>
+      </c>
+      <c r="H84" t="str">
+        <v>ANNUAL FEE</v>
+      </c>
+      <c r="I84" t="str">
+        <v>University of Sindh</v>
+      </c>
+      <c r="J84">
+        <v>42000</v>
+      </c>
+      <c r="K84" t="str">
+        <v>1BILL_PAY</v>
+      </c>
+      <c r="L84" t="str">
+        <v>2024-01-15T19:00:00.000Z</v>
+      </c>
+      <c r="M84" t="str">
+        <v>15:02:00</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>1119376154</v>
+      </c>
+      <c r="B85" t="str">
+        <v>212414107</v>
+      </c>
+      <c r="C85" t="str">
+        <v>ABDUL MOIZ</v>
+      </c>
+      <c r="D85" t="str">
+        <v>JAHANIGIR AHMED</v>
+      </c>
+      <c r="E85" t="str">
+        <v>SHAIKH</v>
+      </c>
+      <c r="F85" t="str">
+        <v>4130397882001</v>
+      </c>
+      <c r="G85" t="str">
+        <v>BS (COMPUTER SCIENCE) PRE-ENGINEERING</v>
+      </c>
+      <c r="H85" t="str">
+        <v>ANNUAL FEE</v>
+      </c>
+      <c r="I85" t="str">
+        <v>University of Sindh</v>
+      </c>
+      <c r="J85">
+        <v>42000</v>
+      </c>
+      <c r="K85" t="str">
+        <v>AGENT</v>
+      </c>
+      <c r="L85" t="str">
+        <v>2024-01-15T19:00:00.000Z</v>
+      </c>
+      <c r="M85" t="str">
+        <v>13:01:00</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>1119784016</v>
+      </c>
+      <c r="B86" t="str">
+        <v>212413654</v>
+      </c>
+      <c r="C86" t="str">
+        <v>AMNA KHANUM</v>
+      </c>
+      <c r="D86" t="str">
+        <v>KASHIF ALI KHAN</v>
+      </c>
+      <c r="E86" t="str">
+        <v>YOUSUFZAI PATHAN</v>
+      </c>
+      <c r="F86" t="str">
+        <v>4410327297538</v>
+      </c>
+      <c r="G86" t="str">
+        <v>BS (ARTIFICIAL INTELLIGENCE)</v>
+      </c>
+      <c r="H86" t="str">
+        <v>ANNUAL FEE</v>
+      </c>
+      <c r="I86" t="str">
+        <v>University of Sindh</v>
+      </c>
+      <c r="J86">
+        <v>42000</v>
+      </c>
+      <c r="K86" t="str">
+        <v>AGENT</v>
+      </c>
+      <c r="L86" t="str">
+        <v>2024-01-15T19:00:00.000Z</v>
+      </c>
+      <c r="M86" t="str">
+        <v>20:08:00</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M79"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M86"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>